<commit_message>
Update genealogy assessment functionality and model rating system. Enhanced the genealogy service to include anonymization mapping for models, updated data structures for assessments, and improved UI components for better user experience. Added comprehensive assessment flow for genealogy and biography evaluations, including saving and loading functionalities. Updated rating categories to include 'Partially Correct' and 'I Don't Know' options.
</commit_message>
<xml_diff>
--- a/Backend/ai_model_ratings.xlsx
+++ b/Backend/ai_model_ratings.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,7 +493,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5b84b348-7592-46a4-9c84-18af78e708d0</t>
+          <t>29ed22c6-3fe6-4816-822f-4a2a7f700f9d</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -513,7 +513,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Albert Einstein — Albert Einstein was a theoretical physicist best known for developing the theory of relativity, which revolutionized the understanding of space, time, and gravity. His most notable contribution, the general theory of relativity, was published in 1915 and remains a cornerstone of modern physics. He also made significant contributions to quantum mechanics, including the explanation of the photoelectric effect, for which he was awarded the Nobel Prize in Physics in 1921. In his later years, Einstein was affiliated with the Institute for Advanced Study in Princeton, New Jersey, where he spent the remainder of his academic career after leaving Germany in 1933 due to the rise of the Nazi regime.</t>
+          <t>Albert Einstein biography assessment</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -523,78 +523,25 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2025-08-27T18:11:27.031Z</t>
+          <t>2025-09-04T08:00:22.137Z</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>f408b463-ea66-49f9-8557-88ca32c09550</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Albert Einstein</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>gpt___5</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>zero-shot</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Albert Einstein — At the Institute for Advanced Study in Princeton from 1933 to 1955, Albert Einstein was a theoretical physicist best known for the general theory of relativity; earlier he held appointments at the University of Berlin and ETH Zurich. His research also established special relativity and advanced quantum theory, including the photoelectric effect, for which he received the 1921 Nobel Prize in Physics.</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Response for gpt___5</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Correct</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Correct</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Correct</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>2025-08-27T18:12:12.529Z</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>